<commit_message>
recording protocol for 3 channels
</commit_message>
<xml_diff>
--- a/EMG_recording_protocol.xlsx
+++ b/EMG_recording_protocol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Desktop\N-pulse\EMG_recording\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Desktop\N-pulse\EMG-Recording\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7433E3-0E60-44CB-87CB-81686105B2CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139806A9-BF6A-4205-B655-076F8E102632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3816" windowWidth="17280" windowHeight="10224" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOFs_of_poses" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="38">
   <si>
     <t>WristExt</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>Sequence4_simple</t>
+  </si>
+  <si>
+    <t>Sequence5_singleDOF</t>
   </si>
 </sst>
 </file>
@@ -461,12 +464,12 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.19921875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.796875" customWidth="1"/>
+    <col min="1" max="1" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>19</v>
       </c>
@@ -489,7 +492,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -515,7 +518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -541,7 +544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -567,7 +570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -593,7 +596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -619,7 +622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -645,7 +648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -671,7 +674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -697,7 +700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -723,7 +726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -749,7 +752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -775,7 +778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -801,7 +804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -827,7 +830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -853,7 +856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -879,7 +882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -905,7 +908,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -931,7 +934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -957,7 +960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -983,7 +986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1009,7 +1012,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>14</v>
       </c>
@@ -1035,7 +1038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -1061,7 +1064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -1087,7 +1090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -1113,7 +1116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>18</v>
       </c>
@@ -1146,19 +1149,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB24CAB7-3A7C-4400-B31B-F77CBCF017C6}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="26.9296875" customWidth="1"/>
-    <col min="4" max="4" width="24.265625" customWidth="1"/>
+    <col min="1" max="3" width="26.88671875" customWidth="1"/>
+    <col min="4" max="4" width="24.21875" customWidth="1"/>
+    <col min="5" max="5" width="23.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1171,8 +1175,11 @@
       <c r="D1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1185,8 +1192,11 @@
       <c r="D2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1199,8 +1209,11 @@
       <c r="D3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1213,8 +1226,11 @@
       <c r="D4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1227,8 +1243,11 @@
       <c r="D5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1241,8 +1260,11 @@
       <c r="D6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1255,8 +1277,11 @@
       <c r="D7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -1269,8 +1294,11 @@
       <c r="D8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1283,8 +1311,11 @@
       <c r="D9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1297,8 +1328,11 @@
       <c r="D10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1312,7 +1346,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1326,7 +1360,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1340,7 +1374,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -1354,42 +1388,42 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -1407,12 +1441,12 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="26.9296875" customWidth="1"/>
+    <col min="1" max="3" width="26.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1423,7 +1457,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1434,7 +1468,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1445,12 +1479,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1458,12 +1492,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1474,7 +1508,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1485,12 +1519,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1498,12 +1532,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1514,7 +1548,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -1522,27 +1556,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>10</v>
       </c>

</xml_diff>